<commit_message>
add results: single, cwm-gpt-3.5
</commit_message>
<xml_diff>
--- a/outputs/errors.xlsx
+++ b/outputs/errors.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuanzhaolin/project/LLM_garment_MES/outputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huanghaolun\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7D94E4-D4F3-254F-BB30-5E97D083041D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB254FC-93B5-406F-911C-5B686D8471D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Question ID</t>
   </si>
@@ -40,36 +39,12 @@
   <si>
     <t>CWM</t>
   </si>
-  <si>
-    <t xml:space="preserve">                                    </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>计算错误</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>错误类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>错误代码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SQL生成错误</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>逻辑链错误</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -80,15 +55,6 @@
     <font>
       <sz val="9"/>
       <name val="等线"/>
-      <family val="4"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -115,11 +81,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -438,20 +401,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.375" customWidth="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -491,7 +454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -511,7 +474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -528,10 +491,10 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -551,7 +514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -571,7 +534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -591,7 +554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -611,7 +574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -631,7 +594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -648,10 +611,10 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -668,10 +631,10 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -691,7 +654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -711,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -730,11 +693,8 @@
       <c r="F14">
         <v>1</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -754,7 +714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -774,7 +734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -794,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -814,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -834,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -854,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -874,7 +834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -894,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -914,7 +874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -934,7 +894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -954,7 +914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -974,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -994,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1014,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1034,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1054,7 +1014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1074,7 +1034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1094,7 +1054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1114,7 +1074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1134,7 +1094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1154,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1174,7 +1134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1194,7 +1154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1214,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1234,7 +1194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1254,7 +1214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1274,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1294,7 +1254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1314,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1334,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1351,10 +1311,10 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1374,7 +1334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1394,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1414,7 +1374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1434,7 +1394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1454,7 +1414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1474,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1494,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1510,11 +1470,11 @@
       <c r="E53">
         <v>0</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="F53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1534,7 +1494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1551,10 +1511,10 @@
         <v>0</v>
       </c>
       <c r="F55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1586,56 +1546,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{510F8920-BBA9-CF46-8A90-06C5DDDD5026}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>